<commit_message>
Hack Request - Pull CPU Goalie Earlier when Losing Addresses #21
</commit_message>
<xml_diff>
--- a/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
+++ b/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\NHL94SNESVault\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57DC557-BE0E-404E-A8D0-7F22CAE017F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB1B2A5-3C0A-40BC-A956-12B1E2200760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="360" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29550" yWindow="555" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAM MAP" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3071" uniqueCount="1389">
   <si>
     <t>Data</t>
   </si>
@@ -4188,13 +4188,40 @@
   </si>
   <si>
     <t>Menu</t>
+  </si>
+  <si>
+    <t>$1630</t>
+  </si>
+  <si>
+    <t>Incremented after each period ends</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Incremented after each period (0 Based)</t>
+  </si>
+  <si>
+    <t>$1790</t>
+  </si>
+  <si>
+    <t>Away Team Score</t>
+  </si>
+  <si>
+    <t>$178E</t>
+  </si>
+  <si>
+    <t>Home Team Score</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4396,6 +4423,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -4652,7 +4686,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4948,6 +4982,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4977,11 +5017,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5737,11 +5780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6567FEA0-CBC9-4D11-BE85-2680A934CDAC}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5763,10 +5806,10 @@
       <c r="C1" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="106" t="s">
         <v>1372</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="105" t="s">
         <v>213</v>
       </c>
     </row>
@@ -5858,101 +5901,89 @@
       <c r="E10" s="49"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
+      <c r="A11" s="48" t="s">
+        <v>1380</v>
+      </c>
       <c r="B11" s="48"/>
       <c r="C11" s="49"/>
       <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="E11" s="49" t="s">
+        <v>1381</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+    </row>
+    <row r="15" spans="1:5" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="118"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
         <v>1354</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B16" s="48" t="s">
         <v>1374</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C16" s="49" t="s">
         <v>1365</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D16" s="49" t="s">
         <v>1369</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E16" s="49" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="48" t="s">
         <v>1355</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="49" t="s">
         <v>1365</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D17" s="49" t="s">
         <v>1369</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E17" s="49" t="s">
         <v>1367</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B18" s="48" t="s">
-        <v>1375</v>
-      </c>
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="49"/>
-      <c r="D18" s="49" t="s">
-        <v>1370</v>
-      </c>
-      <c r="E18" s="49" t="s">
-        <v>1371</v>
-      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>1375</v>
-      </c>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="49"/>
-      <c r="D19" s="49" t="s">
-        <v>1370</v>
-      </c>
-      <c r="E19" s="49" t="s">
-        <v>1376</v>
-      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
@@ -5962,18 +5993,34 @@
       <c r="E20" s="49"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
+      <c r="A21" s="48" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="49" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>1371</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="48" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="D22" s="49" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
@@ -5983,47 +6030,29 @@
       <c r="E23" s="49"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
-      <c r="E24" s="49" t="s">
-        <v>237</v>
-      </c>
+      <c r="E24" s="49"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="48" t="s">
-        <v>240</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
-      <c r="E25" s="49" t="s">
-        <v>238</v>
-      </c>
+      <c r="E25" s="49"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="49"/>
       <c r="D26" s="49"/>
-      <c r="E26" s="49" t="s">
-        <v>242</v>
-      </c>
+      <c r="E26" s="49"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="48" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>1374</v>
@@ -6031,27 +6060,25 @@
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
       <c r="E27" s="49" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="48" t="s">
-        <v>1345</v>
+        <v>240</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>1374</v>
       </c>
       <c r="C28" s="49"/>
-      <c r="D28" s="49" t="s">
-        <v>1377</v>
-      </c>
+      <c r="D28" s="49"/>
       <c r="E28" s="49" t="s">
-        <v>1346</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
-        <v>1347</v>
+        <v>215</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>1374</v>
@@ -6059,12 +6086,12 @@
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
       <c r="E29" s="49" t="s">
-        <v>1378</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="48" t="s">
-        <v>1348</v>
+        <v>216</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>1374</v>
@@ -6072,63 +6099,75 @@
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="49" t="s">
-        <v>1349</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
+      <c r="A31" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>1374</v>
+      </c>
       <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
+      <c r="D31" s="50" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>1383</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>1374</v>
       </c>
-      <c r="C32" s="49" t="s">
-        <v>1360</v>
-      </c>
+      <c r="C32" s="49"/>
       <c r="D32" s="49" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="E32" s="49" t="s">
-        <v>1358</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="48" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>1374</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>1360</v>
-      </c>
-      <c r="D33" s="49" t="s">
-        <v>1379</v>
-      </c>
-      <c r="E33" s="49" t="s">
-        <v>1359</v>
-      </c>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
+      <c r="A34" s="53" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>1375</v>
+      </c>
       <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
+      <c r="D34" s="50" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>1387</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
+      <c r="A35" s="53" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>1375</v>
+      </c>
       <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
+      <c r="D35" s="50" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E35" s="50" t="s">
+        <v>1385</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="48"/>
@@ -6136,6 +6175,108 @@
       <c r="C36" s="49"/>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="48" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="48" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B40" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="48" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B42" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D42" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E42" s="49" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="48" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B43" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E43" s="49" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6158,30 +6299,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="116" t="s">
         <v>1026</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="101"/>
@@ -6641,10 +6782,10 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="115" t="s">
+      <c r="F4" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="106"/>
+      <c r="G4" s="108"/>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
@@ -7690,11 +7831,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="107"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="109"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21143,14 +21284,14 @@
       </c>
     </row>
     <row r="3" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="110" t="s">
         <v>1025</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="108" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="110" t="s">
         <v>1026</v>
       </c>
-      <c r="F3" s="109"/>
+      <c r="F3" s="111"/>
     </row>
     <row r="4" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64" t="s">
@@ -21168,14 +21309,14 @@
       <c r="F4" s="64" t="s">
         <v>1028</v>
       </c>
-      <c r="Y4" s="108" t="s">
+      <c r="Y4" s="110" t="s">
         <v>1025</v>
       </c>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="108" t="s">
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="110" t="s">
         <v>1026</v>
       </c>
-      <c r="AB4" s="109"/>
+      <c r="AB4" s="111"/>
       <c r="AD4" s="63" t="s">
         <v>1029</v>
       </c>
@@ -23319,14 +23460,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="112" t="s">
         <v>1025</v>
       </c>
-      <c r="E3" s="111"/>
-      <c r="F3" s="110" t="s">
+      <c r="E3" s="113"/>
+      <c r="F3" s="112" t="s">
         <v>1026</v>
       </c>
-      <c r="G3" s="111"/>
+      <c r="G3" s="113"/>
     </row>
     <row r="4" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="72" t="s">
@@ -25019,14 +25160,14 @@
   <sheetData>
     <row r="1" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="112" t="s">
         <v>1025</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="110" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="112" t="s">
         <v>1026</v>
       </c>
-      <c r="G2" s="111"/>
+      <c r="G2" s="113"/>
     </row>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="72" t="s">
@@ -25745,17 +25886,17 @@
         <f t="shared" si="2"/>
         <v>D739C</v>
       </c>
-      <c r="I36" s="112" t="s">
+      <c r="I36" s="114" t="s">
         <v>1164</v>
       </c>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
-      <c r="N36" s="111"/>
-      <c r="O36" s="111"/>
-      <c r="P36" s="111"/>
-      <c r="Q36" s="111"/>
+      <c r="J36" s="113"/>
+      <c r="K36" s="113"/>
+      <c r="L36" s="113"/>
+      <c r="M36" s="113"/>
+      <c r="N36" s="113"/>
+      <c r="O36" s="113"/>
+      <c r="P36" s="113"/>
+      <c r="Q36" s="113"/>
     </row>
     <row r="37" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="77" t="s">
@@ -25776,15 +25917,15 @@
         <f t="shared" si="2"/>
         <v>D73BC</v>
       </c>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-      <c r="L37" s="111"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="111"/>
-      <c r="O37" s="111"/>
-      <c r="P37" s="111"/>
-      <c r="Q37" s="111"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="113"/>
+      <c r="L37" s="113"/>
+      <c r="M37" s="113"/>
+      <c r="N37" s="113"/>
+      <c r="O37" s="113"/>
+      <c r="P37" s="113"/>
+      <c r="Q37" s="113"/>
     </row>
     <row r="38" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="76" t="s">
@@ -25805,15 +25946,15 @@
         <f t="shared" si="2"/>
         <v>D73DC</v>
       </c>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
-      <c r="N38" s="111"/>
-      <c r="O38" s="111"/>
-      <c r="P38" s="111"/>
-      <c r="Q38" s="111"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="113"/>
+      <c r="N38" s="113"/>
+      <c r="O38" s="113"/>
+      <c r="P38" s="113"/>
+      <c r="Q38" s="113"/>
     </row>
     <row r="39" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="77" t="s">
@@ -27045,11 +27186,11 @@
       <c r="N1" s="82"/>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="115" t="s">
         <v>1180</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
       <c r="E2" s="83"/>
       <c r="L2" s="82"/>
       <c r="M2" s="82"/>

</xml_diff>

<commit_message>
Hack Request - Pull CPU Goalie Earlier when Losing (#22)
</commit_message>
<xml_diff>
--- a/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
+++ b/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\NHL94SNESVault\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C57DC557-BE0E-404E-A8D0-7F22CAE017F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB1B2A5-3C0A-40BC-A956-12B1E2200760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="360" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29550" yWindow="555" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAM MAP" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3057" uniqueCount="1380">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3071" uniqueCount="1389">
   <si>
     <t>Data</t>
   </si>
@@ -4188,13 +4188,40 @@
   </si>
   <si>
     <t>Menu</t>
+  </si>
+  <si>
+    <t>$1630</t>
+  </si>
+  <si>
+    <t>Incremented after each period ends</t>
+  </si>
+  <si>
+    <t>Period</t>
+  </si>
+  <si>
+    <t>Incremented after each period (0 Based)</t>
+  </si>
+  <si>
+    <t>$1790</t>
+  </si>
+  <si>
+    <t>Away Team Score</t>
+  </si>
+  <si>
+    <t>$178E</t>
+  </si>
+  <si>
+    <t>Home Team Score</t>
+  </si>
+  <si>
+    <t>Score</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="36" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -4396,6 +4423,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="10">
@@ -4652,7 +4686,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="121">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4948,6 +4982,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -4977,11 +5017,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5737,11 +5780,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6567FEA0-CBC9-4D11-BE85-2680A934CDAC}">
-  <dimension ref="A1:E36"/>
+  <dimension ref="A1:E46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K24" sqref="K24"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5763,10 +5806,10 @@
       <c r="C1" s="47" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="117" t="s">
+      <c r="D1" s="106" t="s">
         <v>1372</v>
       </c>
-      <c r="E1" s="116" t="s">
+      <c r="E1" s="105" t="s">
         <v>213</v>
       </c>
     </row>
@@ -5858,101 +5901,89 @@
       <c r="E10" s="49"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="48"/>
+      <c r="A11" s="48" t="s">
+        <v>1380</v>
+      </c>
       <c r="B11" s="48"/>
       <c r="C11" s="49"/>
       <c r="D11" s="49"/>
-      <c r="E11" s="49"/>
+      <c r="E11" s="49" t="s">
+        <v>1381</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="48"/>
+      <c r="A12" s="53"/>
       <c r="B12" s="48"/>
       <c r="C12" s="49"/>
-      <c r="D12" s="49"/>
-      <c r="E12" s="49"/>
+      <c r="D12" s="50"/>
+      <c r="E12" s="50"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="48" t="s">
+      <c r="A13" s="48"/>
+      <c r="B13" s="48"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="48"/>
+      <c r="B14" s="48"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
+      <c r="E14" s="49"/>
+    </row>
+    <row r="15" spans="1:5" s="120" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="118"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="119"/>
+      <c r="D15" s="119"/>
+      <c r="E15" s="119"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="48" t="s">
         <v>1354</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B16" s="48" t="s">
         <v>1374</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C16" s="49" t="s">
         <v>1365</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D16" s="49" t="s">
         <v>1369</v>
       </c>
-      <c r="E13" s="49" t="s">
+      <c r="E16" s="49" t="s">
         <v>1366</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="48" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="48" t="s">
         <v>1355</v>
       </c>
-      <c r="B14" s="48"/>
-      <c r="C14" s="49" t="s">
+      <c r="B17" s="48"/>
+      <c r="C17" s="49" t="s">
         <v>1365</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D17" s="49" t="s">
         <v>1369</v>
       </c>
-      <c r="E14" s="49" t="s">
+      <c r="E17" s="49" t="s">
         <v>1367</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="48"/>
-      <c r="B15" s="48"/>
-      <c r="C15" s="49"/>
-      <c r="D15" s="49"/>
-      <c r="E15" s="49"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="48"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="49"/>
-      <c r="E16" s="49"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="48"/>
-      <c r="B17" s="48"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="49"/>
-      <c r="E17" s="49"/>
-    </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A18" s="48" t="s">
-        <v>1350</v>
-      </c>
-      <c r="B18" s="48" t="s">
-        <v>1375</v>
-      </c>
+      <c r="A18" s="48"/>
+      <c r="B18" s="48"/>
       <c r="C18" s="49"/>
-      <c r="D18" s="49" t="s">
-        <v>1370</v>
-      </c>
-      <c r="E18" s="49" t="s">
-        <v>1371</v>
-      </c>
+      <c r="D18" s="49"/>
+      <c r="E18" s="49"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="48" t="s">
-        <v>1353</v>
-      </c>
-      <c r="B19" s="48" t="s">
-        <v>1375</v>
-      </c>
+      <c r="A19" s="48"/>
+      <c r="B19" s="48"/>
       <c r="C19" s="49"/>
-      <c r="D19" s="49" t="s">
-        <v>1370</v>
-      </c>
-      <c r="E19" s="49" t="s">
-        <v>1376</v>
-      </c>
+      <c r="D19" s="49"/>
+      <c r="E19" s="49"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="48"/>
@@ -5962,18 +5993,34 @@
       <c r="E20" s="49"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="48"/>
-      <c r="B21" s="48"/>
+      <c r="A21" s="48" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B21" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
+      <c r="D21" s="49" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E21" s="49" t="s">
+        <v>1371</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="48"/>
-      <c r="B22" s="48"/>
+      <c r="A22" s="48" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B22" s="48" t="s">
+        <v>1375</v>
+      </c>
       <c r="C22" s="49"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
+      <c r="D22" s="49" t="s">
+        <v>1370</v>
+      </c>
+      <c r="E22" s="49" t="s">
+        <v>1376</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="48"/>
@@ -5983,47 +6030,29 @@
       <c r="E23" s="49"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="B24" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A24" s="48"/>
+      <c r="B24" s="48"/>
       <c r="C24" s="49"/>
       <c r="D24" s="49"/>
-      <c r="E24" s="49" t="s">
-        <v>237</v>
-      </c>
+      <c r="E24" s="49"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="48" t="s">
-        <v>240</v>
-      </c>
-      <c r="B25" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A25" s="48"/>
+      <c r="B25" s="48"/>
       <c r="C25" s="49"/>
       <c r="D25" s="49"/>
-      <c r="E25" s="49" t="s">
-        <v>238</v>
-      </c>
+      <c r="E25" s="49"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="B26" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A26" s="48"/>
+      <c r="B26" s="48"/>
       <c r="C26" s="49"/>
       <c r="D26" s="49"/>
-      <c r="E26" s="49" t="s">
-        <v>242</v>
-      </c>
+      <c r="E26" s="49"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="48" t="s">
-        <v>216</v>
+        <v>239</v>
       </c>
       <c r="B27" s="48" t="s">
         <v>1374</v>
@@ -6031,27 +6060,25 @@
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
       <c r="E27" s="49" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="48" t="s">
-        <v>1345</v>
+        <v>240</v>
       </c>
       <c r="B28" s="48" t="s">
         <v>1374</v>
       </c>
       <c r="C28" s="49"/>
-      <c r="D28" s="49" t="s">
-        <v>1377</v>
-      </c>
+      <c r="D28" s="49"/>
       <c r="E28" s="49" t="s">
-        <v>1346</v>
+        <v>238</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="48" t="s">
-        <v>1347</v>
+        <v>215</v>
       </c>
       <c r="B29" s="48" t="s">
         <v>1374</v>
@@ -6059,12 +6086,12 @@
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
       <c r="E29" s="49" t="s">
-        <v>1378</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="48" t="s">
-        <v>1348</v>
+        <v>216</v>
       </c>
       <c r="B30" s="48" t="s">
         <v>1374</v>
@@ -6072,63 +6099,75 @@
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
       <c r="E30" s="49" t="s">
-        <v>1349</v>
+        <v>243</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="48"/>
-      <c r="B31" s="48"/>
+      <c r="A31" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B31" s="53" t="s">
+        <v>1374</v>
+      </c>
       <c r="C31" s="49"/>
-      <c r="D31" s="49"/>
-      <c r="E31" s="49"/>
+      <c r="D31" s="50" t="s">
+        <v>1382</v>
+      </c>
+      <c r="E31" s="50" t="s">
+        <v>1383</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
-        <v>1356</v>
+        <v>1345</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>1374</v>
       </c>
-      <c r="C32" s="49" t="s">
-        <v>1360</v>
-      </c>
+      <c r="C32" s="49"/>
       <c r="D32" s="49" t="s">
-        <v>1379</v>
+        <v>1377</v>
       </c>
       <c r="E32" s="49" t="s">
-        <v>1358</v>
+        <v>1346</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="48" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B33" s="48" t="s">
-        <v>1374</v>
-      </c>
-      <c r="C33" s="49" t="s">
-        <v>1360</v>
-      </c>
-      <c r="D33" s="49" t="s">
-        <v>1379</v>
-      </c>
-      <c r="E33" s="49" t="s">
-        <v>1359</v>
-      </c>
+      <c r="A33" s="48"/>
+      <c r="B33" s="48"/>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49"/>
+      <c r="E33" s="49"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="48"/>
-      <c r="B34" s="48"/>
+      <c r="A34" s="53" t="s">
+        <v>1386</v>
+      </c>
+      <c r="B34" s="53" t="s">
+        <v>1375</v>
+      </c>
       <c r="C34" s="49"/>
-      <c r="D34" s="49"/>
-      <c r="E34" s="49"/>
+      <c r="D34" s="50" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E34" s="50" t="s">
+        <v>1387</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="48"/>
-      <c r="B35" s="48"/>
+      <c r="A35" s="53" t="s">
+        <v>1384</v>
+      </c>
+      <c r="B35" s="53" t="s">
+        <v>1375</v>
+      </c>
       <c r="C35" s="49"/>
-      <c r="D35" s="49"/>
-      <c r="E35" s="49"/>
+      <c r="D35" s="50" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E35" s="50" t="s">
+        <v>1385</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="48"/>
@@ -6136,6 +6175,108 @@
       <c r="C36" s="49"/>
       <c r="D36" s="49"/>
       <c r="E36" s="49"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="48"/>
+      <c r="B37" s="48"/>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="49"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="48"/>
+      <c r="B38" s="48"/>
+      <c r="C38" s="49"/>
+      <c r="D38" s="49"/>
+      <c r="E38" s="49"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="48" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B39" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C39" s="49"/>
+      <c r="D39" s="49"/>
+      <c r="E39" s="49" t="s">
+        <v>1378</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="48" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B40" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C40" s="49"/>
+      <c r="D40" s="49"/>
+      <c r="E40" s="49" t="s">
+        <v>1349</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" s="48"/>
+      <c r="B41" s="48"/>
+      <c r="C41" s="49"/>
+      <c r="D41" s="49"/>
+      <c r="E41" s="49"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="48" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B42" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C42" s="49" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D42" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E42" s="49" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="48" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B43" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C43" s="49" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D43" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E43" s="49" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="48"/>
+      <c r="B44" s="48"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="49"/>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="48"/>
+      <c r="B45" s="48"/>
+      <c r="C45" s="49"/>
+      <c r="D45" s="49"/>
+      <c r="E45" s="49"/>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" s="48"/>
+      <c r="B46" s="48"/>
+      <c r="C46" s="49"/>
+      <c r="D46" s="49"/>
+      <c r="E46" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6158,30 +6299,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="114" t="s">
+      <c r="B2" s="116" t="s">
         <v>1026</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
-      <c r="E2" s="111"/>
-      <c r="F2" s="111"/>
-      <c r="G2" s="111"/>
-      <c r="H2" s="111"/>
-      <c r="I2" s="111"/>
-      <c r="J2" s="111"/>
-      <c r="K2" s="111"/>
-      <c r="L2" s="111"/>
-      <c r="M2" s="111"/>
-      <c r="N2" s="111"/>
-      <c r="O2" s="111"/>
-      <c r="P2" s="111"/>
-      <c r="Q2" s="111"/>
-      <c r="R2" s="111"/>
-      <c r="S2" s="111"/>
-      <c r="T2" s="111"/>
-      <c r="U2" s="111"/>
-      <c r="V2" s="111"/>
-      <c r="W2" s="111"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
+      <c r="E2" s="113"/>
+      <c r="F2" s="113"/>
+      <c r="G2" s="113"/>
+      <c r="H2" s="113"/>
+      <c r="I2" s="113"/>
+      <c r="J2" s="113"/>
+      <c r="K2" s="113"/>
+      <c r="L2" s="113"/>
+      <c r="M2" s="113"/>
+      <c r="N2" s="113"/>
+      <c r="O2" s="113"/>
+      <c r="P2" s="113"/>
+      <c r="Q2" s="113"/>
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="113"/>
+      <c r="W2" s="113"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="101"/>
@@ -6641,10 +6782,10 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="115" t="s">
+      <c r="F4" s="117" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="106"/>
+      <c r="G4" s="108"/>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
@@ -7690,11 +7831,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="107" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="106"/>
-      <c r="C1" s="107"/>
+      <c r="B1" s="108"/>
+      <c r="C1" s="109"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21143,14 +21284,14 @@
       </c>
     </row>
     <row r="3" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="108" t="s">
+      <c r="C3" s="110" t="s">
         <v>1025</v>
       </c>
-      <c r="D3" s="109"/>
-      <c r="E3" s="108" t="s">
+      <c r="D3" s="111"/>
+      <c r="E3" s="110" t="s">
         <v>1026</v>
       </c>
-      <c r="F3" s="109"/>
+      <c r="F3" s="111"/>
     </row>
     <row r="4" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64" t="s">
@@ -21168,14 +21309,14 @@
       <c r="F4" s="64" t="s">
         <v>1028</v>
       </c>
-      <c r="Y4" s="108" t="s">
+      <c r="Y4" s="110" t="s">
         <v>1025</v>
       </c>
-      <c r="Z4" s="109"/>
-      <c r="AA4" s="108" t="s">
+      <c r="Z4" s="111"/>
+      <c r="AA4" s="110" t="s">
         <v>1026</v>
       </c>
-      <c r="AB4" s="109"/>
+      <c r="AB4" s="111"/>
       <c r="AD4" s="63" t="s">
         <v>1029</v>
       </c>
@@ -23319,14 +23460,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="110" t="s">
+      <c r="D3" s="112" t="s">
         <v>1025</v>
       </c>
-      <c r="E3" s="111"/>
-      <c r="F3" s="110" t="s">
+      <c r="E3" s="113"/>
+      <c r="F3" s="112" t="s">
         <v>1026</v>
       </c>
-      <c r="G3" s="111"/>
+      <c r="G3" s="113"/>
     </row>
     <row r="4" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="72" t="s">
@@ -25019,14 +25160,14 @@
   <sheetData>
     <row r="1" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="110" t="s">
+      <c r="D2" s="112" t="s">
         <v>1025</v>
       </c>
-      <c r="E2" s="111"/>
-      <c r="F2" s="110" t="s">
+      <c r="E2" s="113"/>
+      <c r="F2" s="112" t="s">
         <v>1026</v>
       </c>
-      <c r="G2" s="111"/>
+      <c r="G2" s="113"/>
     </row>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="72" t="s">
@@ -25745,17 +25886,17 @@
         <f t="shared" si="2"/>
         <v>D739C</v>
       </c>
-      <c r="I36" s="112" t="s">
+      <c r="I36" s="114" t="s">
         <v>1164</v>
       </c>
-      <c r="J36" s="111"/>
-      <c r="K36" s="111"/>
-      <c r="L36" s="111"/>
-      <c r="M36" s="111"/>
-      <c r="N36" s="111"/>
-      <c r="O36" s="111"/>
-      <c r="P36" s="111"/>
-      <c r="Q36" s="111"/>
+      <c r="J36" s="113"/>
+      <c r="K36" s="113"/>
+      <c r="L36" s="113"/>
+      <c r="M36" s="113"/>
+      <c r="N36" s="113"/>
+      <c r="O36" s="113"/>
+      <c r="P36" s="113"/>
+      <c r="Q36" s="113"/>
     </row>
     <row r="37" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="77" t="s">
@@ -25776,15 +25917,15 @@
         <f t="shared" si="2"/>
         <v>D73BC</v>
       </c>
-      <c r="I37" s="111"/>
-      <c r="J37" s="111"/>
-      <c r="K37" s="111"/>
-      <c r="L37" s="111"/>
-      <c r="M37" s="111"/>
-      <c r="N37" s="111"/>
-      <c r="O37" s="111"/>
-      <c r="P37" s="111"/>
-      <c r="Q37" s="111"/>
+      <c r="I37" s="113"/>
+      <c r="J37" s="113"/>
+      <c r="K37" s="113"/>
+      <c r="L37" s="113"/>
+      <c r="M37" s="113"/>
+      <c r="N37" s="113"/>
+      <c r="O37" s="113"/>
+      <c r="P37" s="113"/>
+      <c r="Q37" s="113"/>
     </row>
     <row r="38" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="76" t="s">
@@ -25805,15 +25946,15 @@
         <f t="shared" si="2"/>
         <v>D73DC</v>
       </c>
-      <c r="I38" s="111"/>
-      <c r="J38" s="111"/>
-      <c r="K38" s="111"/>
-      <c r="L38" s="111"/>
-      <c r="M38" s="111"/>
-      <c r="N38" s="111"/>
-      <c r="O38" s="111"/>
-      <c r="P38" s="111"/>
-      <c r="Q38" s="111"/>
+      <c r="I38" s="113"/>
+      <c r="J38" s="113"/>
+      <c r="K38" s="113"/>
+      <c r="L38" s="113"/>
+      <c r="M38" s="113"/>
+      <c r="N38" s="113"/>
+      <c r="O38" s="113"/>
+      <c r="P38" s="113"/>
+      <c r="Q38" s="113"/>
     </row>
     <row r="39" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="77" t="s">
@@ -27045,11 +27186,11 @@
       <c r="N1" s="82"/>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="115" t="s">
         <v>1180</v>
       </c>
-      <c r="C2" s="111"/>
-      <c r="D2" s="111"/>
+      <c r="C2" s="113"/>
+      <c r="D2" s="113"/>
       <c r="E2" s="83"/>
       <c r="L2" s="82"/>
       <c r="M2" s="82"/>

</xml_diff>

<commit_message>
Added code samples folder with some samples of other code. Added some missing RAM values to the ROM/RAM mapping excel document
</commit_message>
<xml_diff>
--- a/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
+++ b/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\NHL94SNESVault\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDB1B2A5-3C0A-40BC-A956-12B1E2200760}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D791C30-C8E4-4F8F-A3A1-34C3ADC2A0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29550" yWindow="555" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="555" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAM MAP" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3071" uniqueCount="1389">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3081" uniqueCount="1395">
   <si>
     <t>Data</t>
   </si>
@@ -4193,9 +4193,6 @@
     <t>$1630</t>
   </si>
   <si>
-    <t>Incremented after each period ends</t>
-  </si>
-  <si>
     <t>Period</t>
   </si>
   <si>
@@ -4215,6 +4212,27 @@
   </si>
   <si>
     <t>Score</t>
+  </si>
+  <si>
+    <t>Team Data</t>
+  </si>
+  <si>
+    <t>Incremented after each period ends [0 Based]</t>
+  </si>
+  <si>
+    <t>$1DAB</t>
+  </si>
+  <si>
+    <t>Edit Lines # of Goalies</t>
+  </si>
+  <si>
+    <t>$1DA3</t>
+  </si>
+  <si>
+    <t>Edit Lines # of Players at position (F,D)</t>
+  </si>
+  <si>
+    <t>Edit Lines</t>
   </si>
 </sst>
 </file>
@@ -4988,6 +5006,15 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -5016,15 +5043,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="35" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -5484,9 +5502,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -5524,7 +5542,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -5630,7 +5648,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -5772,7 +5790,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -5780,11 +5798,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6567FEA0-CBC9-4D11-BE85-2680A934CDAC}">
-  <dimension ref="A1:E46"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B29" sqref="B29"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5908,7 +5926,7 @@
       <c r="C11" s="49"/>
       <c r="D11" s="49"/>
       <c r="E11" s="49" t="s">
-        <v>1381</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -5932,12 +5950,12 @@
       <c r="D14" s="49"/>
       <c r="E14" s="49"/>
     </row>
-    <row r="15" spans="1:5" s="120" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="118"/>
-      <c r="B15" s="118"/>
-      <c r="C15" s="119"/>
-      <c r="D15" s="119"/>
-      <c r="E15" s="119"/>
+    <row r="15" spans="1:5" s="109" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="107"/>
+      <c r="B15" s="107"/>
+      <c r="C15" s="108"/>
+      <c r="D15" s="108"/>
+      <c r="E15" s="108"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="48" t="s">
@@ -6037,151 +6055,155 @@
       <c r="E24" s="49"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="48"/>
+      <c r="A25" s="48" t="s">
+        <v>1390</v>
+      </c>
       <c r="B25" s="48"/>
       <c r="C25" s="49"/>
-      <c r="D25" s="49"/>
-      <c r="E25" s="49"/>
+      <c r="D25" s="49" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E25" s="49" t="s">
+        <v>1391</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="48"/>
+      <c r="A26" s="48" t="s">
+        <v>1392</v>
+      </c>
       <c r="B26" s="48"/>
       <c r="C26" s="49"/>
-      <c r="D26" s="49"/>
-      <c r="E26" s="49"/>
+      <c r="D26" s="49" t="s">
+        <v>1394</v>
+      </c>
+      <c r="E26" s="49" t="s">
+        <v>1393</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="48" t="s">
-        <v>239</v>
-      </c>
-      <c r="B27" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A27" s="48"/>
+      <c r="B27" s="48"/>
       <c r="C27" s="49"/>
       <c r="D27" s="49"/>
-      <c r="E27" s="49" t="s">
-        <v>237</v>
-      </c>
+      <c r="E27" s="49"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="48" t="s">
-        <v>240</v>
-      </c>
-      <c r="B28" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A28" s="48"/>
+      <c r="B28" s="48"/>
       <c r="C28" s="49"/>
       <c r="D28" s="49"/>
-      <c r="E28" s="49" t="s">
-        <v>238</v>
-      </c>
+      <c r="E28" s="49"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="48" t="s">
-        <v>215</v>
-      </c>
-      <c r="B29" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A29" s="48"/>
+      <c r="B29" s="48"/>
       <c r="C29" s="49"/>
       <c r="D29" s="49"/>
-      <c r="E29" s="49" t="s">
-        <v>242</v>
-      </c>
+      <c r="E29" s="49"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A30" s="48" t="s">
-        <v>216</v>
-      </c>
-      <c r="B30" s="48" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A30" s="48"/>
+      <c r="B30" s="48"/>
       <c r="C30" s="49"/>
       <c r="D30" s="49"/>
-      <c r="E30" s="49" t="s">
-        <v>243</v>
-      </c>
+      <c r="E30" s="49"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A31" s="48" t="s">
-        <v>1380</v>
-      </c>
-      <c r="B31" s="53" t="s">
-        <v>1374</v>
-      </c>
+      <c r="A31" s="48"/>
+      <c r="B31" s="48"/>
       <c r="C31" s="49"/>
-      <c r="D31" s="50" t="s">
-        <v>1382</v>
-      </c>
-      <c r="E31" s="50" t="s">
-        <v>1383</v>
-      </c>
+      <c r="D31" s="49"/>
+      <c r="E31" s="49"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="48" t="s">
-        <v>1345</v>
+        <v>239</v>
       </c>
       <c r="B32" s="48" t="s">
         <v>1374</v>
       </c>
       <c r="C32" s="49"/>
       <c r="D32" s="49" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E32" s="49" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" s="48" t="s">
+        <v>240</v>
+      </c>
+      <c r="B33" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C33" s="49"/>
+      <c r="D33" s="49" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E33" s="49" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="48" t="s">
+        <v>215</v>
+      </c>
+      <c r="B34" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E34" s="49" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="48" t="s">
+        <v>216</v>
+      </c>
+      <c r="B35" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C35" s="49"/>
+      <c r="D35" s="49" t="s">
+        <v>1388</v>
+      </c>
+      <c r="E35" s="49" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="48" t="s">
+        <v>1380</v>
+      </c>
+      <c r="B36" s="53" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="s">
+        <v>1381</v>
+      </c>
+      <c r="E36" s="50" t="s">
+        <v>1382</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="48" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B37" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C37" s="49"/>
+      <c r="D37" s="49" t="s">
         <v>1377</v>
       </c>
-      <c r="E32" s="49" t="s">
+      <c r="E37" s="49" t="s">
         <v>1346</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A33" s="48"/>
-      <c r="B33" s="48"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49"/>
-      <c r="E33" s="49"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A34" s="53" t="s">
-        <v>1386</v>
-      </c>
-      <c r="B34" s="53" t="s">
-        <v>1375</v>
-      </c>
-      <c r="C34" s="49"/>
-      <c r="D34" s="50" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E34" s="50" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="53" t="s">
-        <v>1384</v>
-      </c>
-      <c r="B35" s="53" t="s">
-        <v>1375</v>
-      </c>
-      <c r="C35" s="49"/>
-      <c r="D35" s="50" t="s">
-        <v>1388</v>
-      </c>
-      <c r="E35" s="50" t="s">
-        <v>1385</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" s="48"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="49"/>
-      <c r="E36" s="49"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" s="48"/>
-      <c r="B37" s="48"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="49"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="48"/>
@@ -6191,29 +6213,33 @@
       <c r="E38" s="49"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" s="48" t="s">
-        <v>1347</v>
-      </c>
-      <c r="B39" s="48" t="s">
-        <v>1374</v>
+      <c r="A39" s="53" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B39" s="53" t="s">
+        <v>1375</v>
       </c>
       <c r="C39" s="49"/>
-      <c r="D39" s="49"/>
-      <c r="E39" s="49" t="s">
-        <v>1378</v>
+      <c r="D39" s="50" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E39" s="50" t="s">
+        <v>1386</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" s="48" t="s">
-        <v>1348</v>
-      </c>
-      <c r="B40" s="48" t="s">
-        <v>1374</v>
+      <c r="A40" s="53" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B40" s="53" t="s">
+        <v>1375</v>
       </c>
       <c r="C40" s="49"/>
-      <c r="D40" s="49"/>
-      <c r="E40" s="49" t="s">
-        <v>1349</v>
+      <c r="D40" s="50" t="s">
+        <v>1387</v>
+      </c>
+      <c r="E40" s="50" t="s">
+        <v>1384</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -6224,52 +6250,44 @@
       <c r="E41" s="49"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" s="48" t="s">
-        <v>1356</v>
-      </c>
-      <c r="B42" s="48" t="s">
+      <c r="A42" s="48"/>
+      <c r="B42" s="48"/>
+      <c r="C42" s="49"/>
+      <c r="D42" s="49"/>
+      <c r="E42" s="49"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="48"/>
+      <c r="B43" s="48"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="49"/>
+      <c r="E43" s="49"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="48" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B44" s="48" t="s">
         <v>1374</v>
       </c>
-      <c r="C42" s="49" t="s">
-        <v>1360</v>
-      </c>
-      <c r="D42" s="49" t="s">
-        <v>1379</v>
-      </c>
-      <c r="E42" s="49" t="s">
-        <v>1358</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" s="48" t="s">
-        <v>1357</v>
-      </c>
-      <c r="B43" s="48" t="s">
-        <v>1374</v>
-      </c>
-      <c r="C43" s="49" t="s">
-        <v>1360</v>
-      </c>
-      <c r="D43" s="49" t="s">
-        <v>1379</v>
-      </c>
-      <c r="E43" s="49" t="s">
-        <v>1359</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" s="48"/>
-      <c r="B44" s="48"/>
       <c r="C44" s="49"/>
       <c r="D44" s="49"/>
-      <c r="E44" s="49"/>
+      <c r="E44" s="49" t="s">
+        <v>1378</v>
+      </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" s="48"/>
-      <c r="B45" s="48"/>
+      <c r="A45" s="48" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B45" s="48" t="s">
+        <v>1374</v>
+      </c>
       <c r="C45" s="49"/>
       <c r="D45" s="49"/>
-      <c r="E45" s="49"/>
+      <c r="E45" s="49" t="s">
+        <v>1349</v>
+      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="48"/>
@@ -6277,6 +6295,61 @@
       <c r="C46" s="49"/>
       <c r="D46" s="49"/>
       <c r="E46" s="49"/>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="48" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B47" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C47" s="49" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D47" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E47" s="49" t="s">
+        <v>1358</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="48" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B48" s="48" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C48" s="49" t="s">
+        <v>1360</v>
+      </c>
+      <c r="D48" s="49" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E48" s="49" t="s">
+        <v>1359</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="48"/>
+      <c r="B49" s="48"/>
+      <c r="C49" s="49"/>
+      <c r="D49" s="49"/>
+      <c r="E49" s="49"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="48"/>
+      <c r="B50" s="48"/>
+      <c r="C50" s="49"/>
+      <c r="D50" s="49"/>
+      <c r="E50" s="49"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51" s="48"/>
+      <c r="B51" s="48"/>
+      <c r="C51" s="49"/>
+      <c r="D51" s="49"/>
+      <c r="E51" s="49"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6299,30 +6372,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:23" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="119" t="s">
         <v>1026</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
-      <c r="E2" s="113"/>
-      <c r="F2" s="113"/>
-      <c r="G2" s="113"/>
-      <c r="H2" s="113"/>
-      <c r="I2" s="113"/>
-      <c r="J2" s="113"/>
-      <c r="K2" s="113"/>
-      <c r="L2" s="113"/>
-      <c r="M2" s="113"/>
-      <c r="N2" s="113"/>
-      <c r="O2" s="113"/>
-      <c r="P2" s="113"/>
-      <c r="Q2" s="113"/>
-      <c r="R2" s="113"/>
-      <c r="S2" s="113"/>
-      <c r="T2" s="113"/>
-      <c r="U2" s="113"/>
-      <c r="V2" s="113"/>
-      <c r="W2" s="113"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
+      <c r="E2" s="116"/>
+      <c r="F2" s="116"/>
+      <c r="G2" s="116"/>
+      <c r="H2" s="116"/>
+      <c r="I2" s="116"/>
+      <c r="J2" s="116"/>
+      <c r="K2" s="116"/>
+      <c r="L2" s="116"/>
+      <c r="M2" s="116"/>
+      <c r="N2" s="116"/>
+      <c r="O2" s="116"/>
+      <c r="P2" s="116"/>
+      <c r="Q2" s="116"/>
+      <c r="R2" s="116"/>
+      <c r="S2" s="116"/>
+      <c r="T2" s="116"/>
+      <c r="U2" s="116"/>
+      <c r="V2" s="116"/>
+      <c r="W2" s="116"/>
     </row>
     <row r="3" spans="2:23" x14ac:dyDescent="0.25">
       <c r="B3" s="101"/>
@@ -6782,10 +6855,10 @@
       <c r="C4" s="1">
         <v>0</v>
       </c>
-      <c r="F4" s="117" t="s">
+      <c r="F4" s="120" t="s">
         <v>183</v>
       </c>
-      <c r="G4" s="108"/>
+      <c r="G4" s="111"/>
     </row>
     <row r="5" spans="1:7" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="20"/>
@@ -7831,11 +7904,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="107" t="s">
+      <c r="A1" s="110" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="108"/>
-      <c r="C1" s="109"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="112"/>
       <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -21284,14 +21357,14 @@
       </c>
     </row>
     <row r="3" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="110" t="s">
+      <c r="C3" s="113" t="s">
         <v>1025</v>
       </c>
-      <c r="D3" s="111"/>
-      <c r="E3" s="110" t="s">
+      <c r="D3" s="114"/>
+      <c r="E3" s="113" t="s">
         <v>1026</v>
       </c>
-      <c r="F3" s="111"/>
+      <c r="F3" s="114"/>
     </row>
     <row r="4" spans="2:30" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="64" t="s">
@@ -21309,14 +21382,14 @@
       <c r="F4" s="64" t="s">
         <v>1028</v>
       </c>
-      <c r="Y4" s="110" t="s">
+      <c r="Y4" s="113" t="s">
         <v>1025</v>
       </c>
-      <c r="Z4" s="111"/>
-      <c r="AA4" s="110" t="s">
+      <c r="Z4" s="114"/>
+      <c r="AA4" s="113" t="s">
         <v>1026</v>
       </c>
-      <c r="AB4" s="111"/>
+      <c r="AB4" s="114"/>
       <c r="AD4" s="63" t="s">
         <v>1029</v>
       </c>
@@ -23460,14 +23533,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="112" t="s">
+      <c r="D3" s="115" t="s">
         <v>1025</v>
       </c>
-      <c r="E3" s="113"/>
-      <c r="F3" s="112" t="s">
+      <c r="E3" s="116"/>
+      <c r="F3" s="115" t="s">
         <v>1026</v>
       </c>
-      <c r="G3" s="113"/>
+      <c r="G3" s="116"/>
     </row>
     <row r="4" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C4" s="72" t="s">
@@ -25160,14 +25233,14 @@
   <sheetData>
     <row r="1" spans="3:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D2" s="112" t="s">
+      <c r="D2" s="115" t="s">
         <v>1025</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="112" t="s">
+      <c r="E2" s="116"/>
+      <c r="F2" s="115" t="s">
         <v>1026</v>
       </c>
-      <c r="G2" s="113"/>
+      <c r="G2" s="116"/>
     </row>
     <row r="3" spans="3:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C3" s="72" t="s">
@@ -25886,17 +25959,17 @@
         <f t="shared" si="2"/>
         <v>D739C</v>
       </c>
-      <c r="I36" s="114" t="s">
+      <c r="I36" s="117" t="s">
         <v>1164</v>
       </c>
-      <c r="J36" s="113"/>
-      <c r="K36" s="113"/>
-      <c r="L36" s="113"/>
-      <c r="M36" s="113"/>
-      <c r="N36" s="113"/>
-      <c r="O36" s="113"/>
-      <c r="P36" s="113"/>
-      <c r="Q36" s="113"/>
+      <c r="J36" s="116"/>
+      <c r="K36" s="116"/>
+      <c r="L36" s="116"/>
+      <c r="M36" s="116"/>
+      <c r="N36" s="116"/>
+      <c r="O36" s="116"/>
+      <c r="P36" s="116"/>
+      <c r="Q36" s="116"/>
     </row>
     <row r="37" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C37" s="77" t="s">
@@ -25917,15 +25990,15 @@
         <f t="shared" si="2"/>
         <v>D73BC</v>
       </c>
-      <c r="I37" s="113"/>
-      <c r="J37" s="113"/>
-      <c r="K37" s="113"/>
-      <c r="L37" s="113"/>
-      <c r="M37" s="113"/>
-      <c r="N37" s="113"/>
-      <c r="O37" s="113"/>
-      <c r="P37" s="113"/>
-      <c r="Q37" s="113"/>
+      <c r="I37" s="116"/>
+      <c r="J37" s="116"/>
+      <c r="K37" s="116"/>
+      <c r="L37" s="116"/>
+      <c r="M37" s="116"/>
+      <c r="N37" s="116"/>
+      <c r="O37" s="116"/>
+      <c r="P37" s="116"/>
+      <c r="Q37" s="116"/>
     </row>
     <row r="38" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C38" s="76" t="s">
@@ -25946,15 +26019,15 @@
         <f t="shared" si="2"/>
         <v>D73DC</v>
       </c>
-      <c r="I38" s="113"/>
-      <c r="J38" s="113"/>
-      <c r="K38" s="113"/>
-      <c r="L38" s="113"/>
-      <c r="M38" s="113"/>
-      <c r="N38" s="113"/>
-      <c r="O38" s="113"/>
-      <c r="P38" s="113"/>
-      <c r="Q38" s="113"/>
+      <c r="I38" s="116"/>
+      <c r="J38" s="116"/>
+      <c r="K38" s="116"/>
+      <c r="L38" s="116"/>
+      <c r="M38" s="116"/>
+      <c r="N38" s="116"/>
+      <c r="O38" s="116"/>
+      <c r="P38" s="116"/>
+      <c r="Q38" s="116"/>
     </row>
     <row r="39" spans="3:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C39" s="77" t="s">
@@ -27186,11 +27259,11 @@
       <c r="N1" s="82"/>
     </row>
     <row r="2" spans="1:16" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="115" t="s">
+      <c r="B2" s="118" t="s">
         <v>1180</v>
       </c>
-      <c r="C2" s="113"/>
-      <c r="D2" s="113"/>
+      <c r="C2" s="116"/>
+      <c r="D2" s="116"/>
       <c r="E2" s="83"/>
       <c r="L2" s="82"/>
       <c r="M2" s="82"/>

</xml_diff>

<commit_message>
Hack Request - Disable Penalty Shots Documented a lot of code and found a lot of RAM addresses and what they do. Fixes #37
</commit_message>
<xml_diff>
--- a/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
+++ b/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\NHL94SNESVault\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D791C30-C8E4-4F8F-A3A1-34C3ADC2A0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E94DA2-CDA4-4FCD-9AF8-CC669900B28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="555" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="555" windowWidth="26655" windowHeight="15000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAM MAP" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3081" uniqueCount="1395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="1398">
   <si>
     <t>Data</t>
   </si>
@@ -4233,6 +4233,15 @@
   </si>
   <si>
     <t>Edit Lines</t>
+  </si>
+  <si>
+    <t>$7E34BC</t>
+  </si>
+  <si>
+    <t>00-04</t>
+  </si>
+  <si>
+    <t>Play Mode Selected - 00 Regular Season; 01 Cont. Playoffs; 02 New Playoffs; 03 Best Of 7; 04 Shootout</t>
   </si>
 </sst>
 </file>
@@ -5800,9 +5809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6567FEA0-CBC9-4D11-BE85-2680A934CDAC}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6345,11 +6354,21 @@
       <c r="E50" s="49"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="48"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
+      <c r="A51" s="48" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B51" s="53" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E51" s="50" t="s">
+        <v>1397</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6364,7 +6383,7 @@
   </sheetPr>
   <dimension ref="B2:W64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>

<commit_message>
Hack Request - Disable Penalty Shots (#39)
</commit_message>
<xml_diff>
--- a/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
+++ b/Docs/SNES NHL94 ROM-RAM Mapping Project.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Personal\NHL94SNESVault\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D791C30-C8E4-4F8F-A3A1-34C3ADC2A0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28E94DA2-CDA4-4FCD-9AF8-CC669900B28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="555" windowWidth="26655" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1455" yWindow="555" windowWidth="26655" windowHeight="15000" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RAM MAP" sheetId="6" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3081" uniqueCount="1395">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3086" uniqueCount="1398">
   <si>
     <t>Data</t>
   </si>
@@ -4233,6 +4233,15 @@
   </si>
   <si>
     <t>Edit Lines</t>
+  </si>
+  <si>
+    <t>$7E34BC</t>
+  </si>
+  <si>
+    <t>00-04</t>
+  </si>
+  <si>
+    <t>Play Mode Selected - 00 Regular Season; 01 Cont. Playoffs; 02 New Playoffs; 03 Best Of 7; 04 Shootout</t>
   </si>
 </sst>
 </file>
@@ -5800,9 +5809,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6567FEA0-CBC9-4D11-BE85-2680A934CDAC}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -6345,11 +6354,21 @@
       <c r="E50" s="49"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A51" s="48"/>
-      <c r="B51" s="48"/>
-      <c r="C51" s="49"/>
-      <c r="D51" s="49"/>
-      <c r="E51" s="49"/>
+      <c r="A51" s="48" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B51" s="53" t="s">
+        <v>1374</v>
+      </c>
+      <c r="C51" s="50" t="s">
+        <v>1396</v>
+      </c>
+      <c r="D51" s="50" t="s">
+        <v>1379</v>
+      </c>
+      <c r="E51" s="50" t="s">
+        <v>1397</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6364,7 +6383,7 @@
   </sheetPr>
   <dimension ref="B2:W64"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>